<commit_message>
Creating  objects and editing functions
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DB27BC-10E2-4F63-9A85-E3071BE2A97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1D5107-2052-425F-A256-6D05B312E181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>Parameter</t>
   </si>
@@ -101,9 +101,6 @@
     <t>wye</t>
   </si>
   <si>
-    <t>dataset/pv_df</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
@@ -113,9 +110,6 @@
     <t>yyyy-mm-dd HH:mn</t>
   </si>
   <si>
-    <t>0.8</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -141,6 +135,9 @@
   </si>
   <si>
     <t>Emin(%)</t>
+  </si>
+  <si>
+    <t>dados_power_ajustado</t>
   </si>
 </sst>
 </file>
@@ -150,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -249,6 +246,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -272,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -290,14 +295,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -537,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,7 +554,7 @@
         <v>41096.5</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -556,10 +562,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41097.5</v>
+        <v>41096.520833333336</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,7 +576,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -586,14 +592,14 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -601,7 +607,7 @@
       <c r="C1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -613,8 +619,8 @@
       <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="16" t="s">
-        <v>34</v>
+      <c r="H1" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>8</v>
@@ -627,19 +633,22 @@
       <c r="B2" s="5">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
       <c r="D2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="5">
-        <v>1000</v>
+        <v>10</v>
       </c>
       <c r="F2" s="5">
-        <v>260</v>
+        <v>15</v>
       </c>
       <c r="G2" s="5">
-        <v>1275</v>
-      </c>
-      <c r="H2" s="17">
+        <v>30</v>
+      </c>
+      <c r="H2" s="16">
         <v>20</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -647,30 +656,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3">
-        <v>0.5</v>
-      </c>
-      <c r="F3">
-        <v>400</v>
-      </c>
-      <c r="G3">
-        <v>1500</v>
-      </c>
-      <c r="H3" s="18">
-        <v>15</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>25</v>
-      </c>
+      <c r="D3" s="11"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="11"/>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
@@ -689,14 +677,17 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -746,13 +737,13 @@
         <v>20</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2">
         <v>123</v>
@@ -771,9 +762,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -781,7 +772,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>10</v>
@@ -795,8 +786,8 @@
       <c r="E1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>14</v>
+      <c r="F1" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>15</v>
@@ -805,10 +796,10 @@
         <v>16</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>18</v>
@@ -817,7 +808,7 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -835,7 +826,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -844,18 +835,18 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
-      </c>
-      <c r="K2" s="15">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="K2" s="19">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -870,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3">
         <v>8</v>
@@ -879,18 +870,18 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="15">
-        <v>13</v>
+        <v>29</v>
+      </c>
+      <c r="K3" s="19">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -905,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -914,9 +905,9 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="15">
+        <v>29</v>
+      </c>
+      <c r="K4" s="19">
         <v>12</v>
       </c>
     </row>
@@ -927,7 +918,11 @@
       <c r="K6" s="10"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="10"/>
       <c r="K8" s="14"/>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I9" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>

</xml_diff>

<commit_message>
Correction of bus name in functions
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1D5107-2052-425F-A256-6D05B312E181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEF7382-1284-4F5D-A37B-42028D5AD250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -592,7 +592,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -676,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Modify the functions to return dataframes with informations
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEF7382-1284-4F5D-A37B-42028D5AD250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC712359-7518-4B32-8904-1390C8D37966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-132" yWindow="-132" windowWidth="23304" windowHeight="13224" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -525,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -676,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Change some functions and add another methods
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EBF40F-2FFD-4815-90F2-C8448BAC2729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ECD62B-FE59-4450-9BDF-77EC5F533AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30840" yWindow="-8700" windowWidth="30960" windowHeight="19440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30840" yWindow="-8700" windowWidth="30960" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
     <t>Emin(%)</t>
   </si>
   <si>
-    <t>dados_power_ajustado</t>
+    <t>pv_generation_norm</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -535,7 +535,7 @@
     <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -546,7 +546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -557,7 +557,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -568,7 +568,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -680,8 +680,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add function to plot and modify powerflow
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86ECD62B-FE59-4450-9BDF-77EC5F533AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5A630A-8E3C-43E1-B205-1F59FC2AEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30840" yWindow="-8700" windowWidth="30960" windowHeight="19440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5830" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -525,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3">
-        <v>41096.5</v>
+        <v>41097.25</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>23</v>
@@ -562,7 +562,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41097.5</v>
+        <v>41098.25</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>23</v>
@@ -680,7 +680,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Funçao plot e switch
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5A630A-8E3C-43E1-B205-1F59FC2AEA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33619A9-1BEC-47AC-8067-A733A63DD4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-5830" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5830" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -525,7 +525,7 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -595,8 +595,8 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -681,7 +681,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Atualização do main e definição da função de operação da bateria
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CD991F-3A77-4710-854E-BBF1CA4CD4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048006E9-EEB2-426D-9427-B43760F86F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -137,7 +137,7 @@
     <t>Emin(%)</t>
   </si>
   <si>
-    <t>pv_generation_norm</t>
+    <t>pv_generation</t>
   </si>
 </sst>
 </file>
@@ -525,8 +525,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -596,7 +596,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="5">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="G2" s="5">
         <v>30</v>
@@ -680,8 +680,8 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -729,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Atualização do fluxo de potência e função da bateria. Modularização do Main
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048006E9-EEB2-426D-9427-B43760F86F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BB8CF87-EE63-4FCD-88ED-8D8FF04A86E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37470" yWindow="-4660" windowWidth="28800" windowHeight="15950" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Parameter</t>
   </si>
@@ -56,12 +56,6 @@
     <t>Pmax</t>
   </si>
   <si>
-    <t>Einit</t>
-  </si>
-  <si>
-    <t>Emax</t>
-  </si>
-  <si>
     <t>Efficiency</t>
   </si>
   <si>
@@ -134,10 +128,19 @@
     <t>MAC003996</t>
   </si>
   <si>
-    <t>Emin(%)</t>
-  </si>
-  <si>
     <t>pv_generation</t>
+  </si>
+  <si>
+    <t>Einit(%)</t>
+  </si>
+  <si>
+    <t>SOC_min(%)</t>
+  </si>
+  <si>
+    <t>SOC_max(%)</t>
+  </si>
+  <si>
+    <t>Cmax</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -554,7 +557,7 @@
         <v>41097.25</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -565,7 +568,7 @@
         <v>41098.25</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -576,7 +579,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -593,44 +596,51 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>12</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="I1" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -641,7 +651,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="5">
         <v>10</v>
@@ -653,18 +663,21 @@
         <v>30</v>
       </c>
       <c r="H2" s="16">
-        <v>20</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="I2" s="16">
+        <v>90</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="11"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J3" s="11"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
     </row>
   </sheetData>
@@ -680,7 +693,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -691,34 +704,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -732,10 +745,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2">
         <v>20</v>
@@ -747,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2">
         <v>123</v>
@@ -776,43 +789,43 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>16</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -821,16 +834,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -839,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K2" s="19">
         <v>12</v>
@@ -847,7 +860,7 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -856,16 +869,16 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H3">
         <v>8</v>
@@ -874,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K3" s="19">
         <v>12</v>
@@ -882,7 +895,7 @@
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -891,16 +904,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -909,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K4" s="19">
         <v>12</v>

</xml_diff>

<commit_message>
Alteração da função para adicionar a bateria em cada barramento
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEB54DE-FD7F-405D-B557-62D9DDF537A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BF1011-1118-4BA5-BEF9-B5F54D7162A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37470" yWindow="-4660" windowWidth="28800" windowHeight="15950" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -598,8 +598,8 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -693,7 +693,7 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Atualização dos arquivos das funções
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BF1011-1118-4BA5-BEF9-B5F54D7162A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB8C690-9665-4429-8C96-BE9892D3C446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-5700" windowWidth="38620" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-36890" yWindow="-4080" windowWidth="28800" windowHeight="15950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
   <si>
     <t>Parameter</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Conn</t>
   </si>
   <si>
-    <t>kW</t>
-  </si>
-  <si>
     <t>Pf</t>
   </si>
   <si>
@@ -113,21 +110,12 @@
     <t>Vminpu</t>
   </si>
   <si>
-    <t>MAC003982</t>
-  </si>
-  <si>
     <t>0.9</t>
   </si>
   <si>
     <t>0.92</t>
   </si>
   <si>
-    <t>MAC003983</t>
-  </si>
-  <si>
-    <t>MAC003996</t>
-  </si>
-  <si>
     <t>pv_generation</t>
   </si>
   <si>
@@ -141,6 +129,30 @@
   </si>
   <si>
     <t>Cmax</t>
+  </si>
+  <si>
+    <t>MAC003982.csv</t>
+  </si>
+  <si>
+    <t>MAC003983.csv</t>
+  </si>
+  <si>
+    <t>MAC003996.csv</t>
+  </si>
+  <si>
+    <t>MAC003997.csv</t>
+  </si>
+  <si>
+    <t>0.93</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>MAC003998.csv</t>
+  </si>
+  <si>
+    <t>0.96</t>
   </si>
 </sst>
 </file>
@@ -162,12 +174,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -175,23 +189,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -199,6 +217,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -236,11 +255,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -526,9 +547,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -546,7 +567,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -557,7 +578,7 @@
         <v>41097.25</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -568,7 +589,7 @@
         <v>41098.25</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
@@ -579,11 +600,14 @@
         <v>30</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -598,7 +622,7 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -610,7 +634,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
@@ -625,16 +649,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>6</v>
@@ -651,7 +675,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="5">
         <v>10</v>
@@ -694,7 +718,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -704,7 +728,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
@@ -719,19 +743,19 @@
         <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -739,19 +763,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F2" s="2">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -760,7 +784,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J2" s="2">
         <v>123</v>
@@ -782,14 +806,17 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:K8"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>8</v>
@@ -807,25 +834,25 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>14</v>
-      </c>
       <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="K1" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L1" s="4"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -834,16 +861,16 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -852,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K2" s="19">
         <v>12</v>
@@ -860,7 +887,7 @@
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -869,16 +896,16 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>26</v>
+      <c r="G3" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="H3">
         <v>8</v>
@@ -887,15 +914,15 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K3" s="19">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -904,16 +931,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>26</v>
+      <c r="G4" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -922,17 +949,81 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="K4" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="19">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K5" s="10"/>
-    </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K6" s="10"/>
+      <c r="A6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="19">
+        <v>23</v>
+      </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="10"/>

</xml_diff>

<commit_message>
Manage load and generation_files, and reorganize bus_voltage function
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBB8C690-9665-4429-8C96-BE9892D3C446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3537B4DA-B25A-481C-BC98-10B11B430FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-36890" yWindow="-4080" windowWidth="28800" windowHeight="15950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -550,13 +550,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.8" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41098.25</v>
+        <v>41462.270833333336</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>20</v>
@@ -604,7 +604,9 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10"/>
@@ -623,7 +625,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -718,7 +720,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -806,7 +808,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Run Simulations of power flow
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3537B4DA-B25A-481C-BC98-10B11B430FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6025CF5A-E9B2-4297-9527-7ACB3425D558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41462.270833333336</v>
+        <v>41462.25</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Create a Public Ilumination Profile
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6025CF5A-E9B2-4297-9527-7ACB3425D558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6866DCC4-AF8A-4898-855C-C07CC4C78345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41462.25</v>
+        <v>41098.25</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Função para adicionar iluminação pública
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6866DCC4-AF8A-4898-855C-C07CC4C78345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61AEE81B-27EA-47BF-B7BB-8B16C88A05F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
     <sheet name="BESS" sheetId="2" r:id="rId2"/>
     <sheet name="Generator" sheetId="3" r:id="rId3"/>
     <sheet name="Load" sheetId="4" r:id="rId4"/>
+    <sheet name="Public_Ilumination" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="44">
   <si>
     <t>Parameter</t>
   </si>
@@ -153,6 +154,21 @@
   </si>
   <si>
     <t>0.96</t>
+  </si>
+  <si>
+    <t>kW</t>
+  </si>
+  <si>
+    <t>0.084</t>
+  </si>
+  <si>
+    <t>pub_ilum</t>
+  </si>
+  <si>
+    <t>0.9823</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -162,7 +178,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -277,6 +293,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -549,7 +570,7 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
@@ -808,7 +829,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1038,4 +1059,237 @@
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3425D832-8626-4E16-B86F-D606408C1A89}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="16" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modificações nos arquivos .dss
</commit_message>
<xml_diff>
--- a/data/spreadsheets/teste_sheet.xlsx
+++ b/data/spreadsheets/teste_sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Code\GridFlexPy\data\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao9\GitHub\GridFlexPy\data\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD48212-9AAF-45E9-9D83-7C90122E3251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60451D7D-1894-47B7-B087-B533B1C0A770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="48">
   <si>
     <t>Parameter</t>
   </si>
@@ -117,9 +117,6 @@
     <t>0.92</t>
   </si>
   <si>
-    <t>pv_generation</t>
-  </si>
-  <si>
     <t>Einit(%)</t>
   </si>
   <si>
@@ -156,12 +153,6 @@
     <t>0.96</t>
   </si>
   <si>
-    <t>kW</t>
-  </si>
-  <si>
-    <t>0.084</t>
-  </si>
-  <si>
     <t>pub_ilum</t>
   </si>
   <si>
@@ -169,6 +160,27 @@
   </si>
   <si>
     <t>delta</t>
+  </si>
+  <si>
+    <t>pv_generation.csv</t>
+  </si>
+  <si>
+    <t>MAC003982</t>
+  </si>
+  <si>
+    <t>MAC003983</t>
+  </si>
+  <si>
+    <t>MAC003996</t>
+  </si>
+  <si>
+    <t>MAC003997</t>
+  </si>
+  <si>
+    <t>MAC003998</t>
+  </si>
+  <si>
+    <t>pub_ilum.csv</t>
   </si>
 </sst>
 </file>
@@ -571,7 +583,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -607,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3">
-        <v>41462.25</v>
+        <v>41098.270833333336</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>20</v>
@@ -672,16 +684,16 @@
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>6</v>
@@ -741,7 +753,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -807,7 +819,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="J2" s="2">
         <v>123</v>
@@ -829,12 +841,13 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -871,11 +884,13 @@
       <c r="K1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="4"/>
+      <c r="L1" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -907,10 +922,13 @@
       <c r="K2" s="19">
         <v>12</v>
       </c>
+      <c r="L2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -928,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3">
         <v>8</v>
@@ -942,10 +960,13 @@
       <c r="K3" s="19">
         <v>23</v>
       </c>
+      <c r="L3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -977,10 +998,13 @@
       <c r="K4" s="19">
         <v>13</v>
       </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -998,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5">
         <v>8</v>
@@ -1012,10 +1036,13 @@
       <c r="K5" s="19">
         <v>12</v>
       </c>
+      <c r="L5" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1033,7 +1060,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6">
         <v>8</v>
@@ -1042,10 +1069,13 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K6" s="19">
         <v>23</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1063,19 +1093,20 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3425D832-8626-4E16-B86F-D606408C1A89}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
@@ -1092,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>12</v>
@@ -1106,13 +1137,16 @@
       <c r="J1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1121,16 +1155,16 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>40</v>
+      <c r="F2">
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H2">
         <v>8</v>
@@ -1141,31 +1175,34 @@
       <c r="J2" t="s">
         <v>25</v>
       </c>
-      <c r="K2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="19">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>40</v>
+      <c r="F3">
+        <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H3">
         <v>8</v>
@@ -1176,31 +1213,34 @@
       <c r="J3" t="s">
         <v>25</v>
       </c>
-      <c r="K3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="19">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="F4" t="s">
-        <v>40</v>
+      <c r="F4">
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H4">
         <v>8</v>
@@ -1211,31 +1251,34 @@
       <c r="J4" t="s">
         <v>25</v>
       </c>
-      <c r="K4">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="19">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>16</v>
       </c>
-      <c r="F5" t="s">
-        <v>40</v>
+      <c r="F5">
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H5">
         <v>8</v>
@@ -1246,31 +1289,34 @@
       <c r="J5" t="s">
         <v>25</v>
       </c>
-      <c r="K5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="19">
+        <v>23</v>
+      </c>
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
-        <v>40</v>
+      <c r="F6">
+        <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H6">
         <v>8</v>
@@ -1281,11 +1327,17 @@
       <c r="J6" t="s">
         <v>25</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="19">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" s="19"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
     </row>
   </sheetData>

</xml_diff>